<commit_message>
Some figures has been redrawed.
</commit_message>
<xml_diff>
--- a/Figures/Structure_randomForest/RF_Phase_Real_pred.xlsx
+++ b/Figures/Structure_randomForest/RF_Phase_Real_pred.xlsx
@@ -12,7 +12,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="140">
+  <si>
+    <t>ID</t>
+  </si>
   <si>
     <t>Alloy_System</t>
   </si>
@@ -23,7 +26,7 @@
     <t>observed</t>
   </si>
   <si>
-    <t>predicated</t>
+    <t>predicted</t>
   </si>
   <si>
     <t>1</t>
@@ -179,78 +182,102 @@
     <t>51</t>
   </si>
   <si>
+    <t>Cu-Ni-Al-Co-Cr-Fe</t>
+  </si>
+  <si>
+    <t>Ti-V-Cr-Zr-Hf</t>
+  </si>
+  <si>
+    <t>Fe-Co-Ni-Zr-Cu-Al-V</t>
+  </si>
+  <si>
+    <t>Al-Co-Cr-Fe-Mo-Ni</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cu-Co-Ni-Cr-Al-Fe</t>
+  </si>
+  <si>
+    <t>Al-Co-Cr-Cu-Fe-Ni-V</t>
+  </si>
+  <si>
+    <t>Cu-Ni-Al-Co-Cr</t>
+  </si>
+  <si>
+    <t>Cu-Ni-Co-Zn-Al-Ti</t>
+  </si>
+  <si>
+    <t>Al-Ti-Ni-Mn-B</t>
+  </si>
+  <si>
+    <t>Fe-Co-Cr-Ni-Al</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Nb-Mo-Ta-W</t>
+  </si>
+  <si>
+    <t>V-Nb-Mo-Ta-W</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fe-Ni-Co-Si-Cr-Al-Ti </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ta-Nb-Hf-Zr-Ti </t>
+  </si>
+  <si>
+    <t>Ti-Zr-Nb-Mo-V</t>
+  </si>
+  <si>
+    <t>Mn-Cr-Fe-Ni-Al</t>
+  </si>
+  <si>
+    <t>Al-Co-Cr-Fe-Mo</t>
+  </si>
+  <si>
+    <t>Co-Cr-Fe -Ni-Al-Mo</t>
+  </si>
+  <si>
+    <t>Ti-Co-Cr-Fe-Ni-Cu-Al</t>
+  </si>
+  <si>
+    <t>Zr-Hf-Ti-Cu-Co</t>
+  </si>
+  <si>
     <t xml:space="preserve">Al-Li-Mg-Sc-Ti </t>
   </si>
   <si>
-    <t xml:space="preserve"> Cu-Co-Ni-Cr-Al-Fe</t>
-  </si>
-  <si>
-    <t>Al-Co-Cr-Cu-Fe-Ni-V</t>
-  </si>
-  <si>
     <t>Cu-Ni-Al-Co</t>
   </si>
   <si>
-    <t>Cu-Ni-Al-Co-Cr</t>
-  </si>
-  <si>
-    <t>Cu-Ni-Al-Co-Cr-Fe</t>
+    <t>Cu-Ni-Co</t>
+  </si>
+  <si>
+    <t>Co-Cr-Fe-Ni-Al</t>
+  </si>
+  <si>
+    <t>Fe-Co-Cr-Ni</t>
+  </si>
+  <si>
+    <t>Fe-Co-Cr-Ni-Pd</t>
+  </si>
+  <si>
+    <t>Co-Cr-Fe-Ni-Mn-Cu</t>
+  </si>
+  <si>
+    <t>Ti-Co-Cr-Fe-Ni-Cu</t>
+  </si>
+  <si>
+    <t>Ti -Co-Cr-Fe-Ni-Cu-Al</t>
+  </si>
+  <si>
+    <t>Mn-Cr-Fe-Ni-Cu</t>
   </si>
   <si>
     <t>Al-Co-Cr-Cu-Fe-Ni</t>
   </si>
   <si>
-    <t>Ti-V-Cr-Zr-Hf</t>
-  </si>
-  <si>
-    <t>Fe-Co-Ni-Zr-Cu-Al-V</t>
-  </si>
-  <si>
-    <t>Cu-Ni-Co-Zn-Al-Ti</t>
-  </si>
-  <si>
-    <t>Al-Ti-Ni-Mn-B</t>
-  </si>
-  <si>
     <t>Fe-Ni-Cr-Cu-Al</t>
   </si>
   <si>
-    <t>Al-Co-Cr-Fe-Mo</t>
-  </si>
-  <si>
-    <t>Cu-Ni-Co</t>
-  </si>
-  <si>
-    <t>Co-Cr-Fe-Ni-Al</t>
-  </si>
-  <si>
-    <t>Fe-Co-Cr-Ni</t>
-  </si>
-  <si>
-    <t>Fe-Co-Cr-Ni-Pd</t>
-  </si>
-  <si>
-    <t>Fe-Co-Cr-Ni-Al</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Nb-Mo-Ta-W</t>
-  </si>
-  <si>
-    <t>V-Nb-Mo-Ta-W</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fe-Ni-Co-Si-Cr-Al-Ti </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ta-Nb-Hf-Zr-Ti </t>
-  </si>
-  <si>
-    <t>Al-Co-Cr-Fe-Mo-Ni</t>
-  </si>
-  <si>
-    <t>Ti-Zr-Nb-Mo-V</t>
-  </si>
-  <si>
     <t>Ni-Co-Cr-Fe</t>
   </si>
   <si>
@@ -263,40 +290,64 @@
     <t>Co-Cr-Fe-Ni-Mn-Ge</t>
   </si>
   <si>
-    <t>Co-Cr-Fe-Ni-Mn-Cu</t>
-  </si>
-  <si>
     <t>Co-Cr-Ni-Cu-Al</t>
   </si>
   <si>
-    <t>Ti-Co-Cr-Fe-Ni-Cu</t>
-  </si>
-  <si>
     <t>Ti-Co-Cr-Fe-Ni-Al</t>
   </si>
   <si>
-    <t>Ti -Co-Cr-Fe-Ni-Cu-Al</t>
-  </si>
-  <si>
-    <t>Ti-Co-Cr-Fe-Ni-Cu-Al</t>
-  </si>
-  <si>
-    <t>Mn-Cr-Fe-Ni-Al</t>
-  </si>
-  <si>
-    <t>Mn-Cr-Fe-Ni-Cu</t>
-  </si>
-  <si>
     <t>Mn -Cr-Fe-Ni-Cu</t>
   </si>
   <si>
     <t>Co-Cr-Fe-Ni-Cu-Al-V</t>
   </si>
   <si>
-    <t>Co-Cr-Fe -Ni-Al-Mo</t>
-  </si>
-  <si>
-    <t>Zr-Hf-Ti-Cu-Co</t>
+    <t>Cu0.5-Ni-Al-Co-Cr-Fe</t>
+  </si>
+  <si>
+    <t>Al-Co-Cr1.5-Fe-Mo0.5-Ni</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cu-Co-Ni-Cr-Al2.8-Fe</t>
+  </si>
+  <si>
+    <t>Al0.5-Co-Cr-Cu-Fe-Ni-V1.8</t>
+  </si>
+  <si>
+    <t>Cu0.5-Ni-Al-Co-Cr</t>
+  </si>
+  <si>
+    <t>Al-Ti-Ni-Mn-B0.1</t>
+  </si>
+  <si>
+    <t>Al-Ti-Ni-Mn-B0.4</t>
+  </si>
+  <si>
+    <t>Fe-Co-Cr-Ni-Al2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Nb25-Mo25-Ta25-W25</t>
+  </si>
+  <si>
+    <t>V20-Nb20-Mo20-Ta20-W20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fe6-Ni-Co-Si-Cr-Al-Ti </t>
+  </si>
+  <si>
+    <t>Ti-Zr-Nb-Mo-V3</t>
+  </si>
+  <si>
+    <t>Mn-Cr-Fe1.5-Ni0.5-Al0.3</t>
+  </si>
+  <si>
+    <t>Al-Co-Cr-Fe1.0-Mo0.5</t>
+  </si>
+  <si>
+    <t>Co-Cr-Fe0.6 -Ni-Al-Mo0.5</t>
+  </si>
+  <si>
+    <t>Ti0.5-Co-Cr-Fe-Ni-Cu0.25-Al</t>
   </si>
   <si>
     <t xml:space="preserve">Al20-Li20-Mg10-Sc20-Ti30 </t>
@@ -305,60 +356,33 @@
     <t xml:space="preserve"> Cu-Co-Ni-Cr-Al0.5-Fe</t>
   </si>
   <si>
-    <t xml:space="preserve"> Cu-Co-Ni-Cr-Al2.8-Fe</t>
+    <t>Cu0.5-Ni-Al-Co</t>
+  </si>
+  <si>
+    <t>Co-Cr-Fe-Ni-Al0.3</t>
+  </si>
+  <si>
+    <t>Fe-Co-Cr-Ni-Pd2</t>
+  </si>
+  <si>
+    <t>Ti0.5-Co-Cr-Fe-Ni-Cu</t>
+  </si>
+  <si>
+    <t>Ti0.5 -Co-Cr-Fe-Ni-Cu0.75-Al0.25</t>
+  </si>
+  <si>
+    <t>Co-Cr-Fe-Ni-Al0.375</t>
+  </si>
+  <si>
+    <t>Mn-Cr-Fe2-Ni2-Cu2</t>
   </si>
   <si>
     <t>Al0.5-Co-Cr-Cu-Fe-Ni-V0.6</t>
   </si>
   <si>
-    <t>Al0.5-Co-Cr-Cu-Fe-Ni-V1.8</t>
-  </si>
-  <si>
-    <t>Cu0.5-Ni-Al-Co</t>
-  </si>
-  <si>
-    <t>Cu0.5-Ni-Al-Co-Cr</t>
-  </si>
-  <si>
-    <t>Cu0.5-Ni-Al-Co-Cr-Fe</t>
-  </si>
-  <si>
     <t>Al-Co-Cr-Cu-Fe-Ni0.5</t>
   </si>
   <si>
-    <t>Al-Ti-Ni-Mn-B0.1</t>
-  </si>
-  <si>
-    <t>Al-Ti-Ni-Mn-B0.4</t>
-  </si>
-  <si>
-    <t>Al-Co-Cr-Fe1.0-Mo0.5</t>
-  </si>
-  <si>
-    <t>Co-Cr-Fe-Ni-Al0.3</t>
-  </si>
-  <si>
-    <t>Fe-Co-Cr-Ni-Pd2</t>
-  </si>
-  <si>
-    <t>Fe-Co-Cr-Ni-Al2</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Nb25-Mo25-Ta25-W25</t>
-  </si>
-  <si>
-    <t>V20-Nb20-Mo20-Ta20-W20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fe6-Ni-Co-Si-Cr-Al-Ti </t>
-  </si>
-  <si>
-    <t>Al-Co-Cr1.5-Fe-Mo0.5-Ni</t>
-  </si>
-  <si>
-    <t>Ti-Zr-Nb-Mo-V3</t>
-  </si>
-  <si>
     <t>Co-Cr-Fe-Ni-Cu-Al1.5</t>
   </si>
   <si>
@@ -368,64 +392,43 @@
     <t>Co-Cr0.5-Fe-Ni-Cu-Al</t>
   </si>
   <si>
-    <t>Ti0.5-Co-Cr-Fe-Ni-Cu</t>
-  </si>
-  <si>
     <t>Ti0.5-Co3-Cr-Fe-Ni-Al</t>
   </si>
   <si>
-    <t>Ti0.5 -Co-Cr-Fe-Ni-Cu0.75-Al0.25</t>
-  </si>
-  <si>
-    <t>Ti0.5-Co-Cr-Fe-Ni-Cu0.25-Al</t>
-  </si>
-  <si>
-    <t>Co-Cr-Fe-Ni-Al0.375</t>
-  </si>
-  <si>
-    <t>Mn-Cr-Fe1.5-Ni0.5-Al0.3</t>
-  </si>
-  <si>
     <t>Mn-Cr2-Fe2-Ni-Cu</t>
   </si>
   <si>
     <t>Mn2 -Cr-Fe2-Ni-Cu2</t>
   </si>
   <si>
-    <t>Mn-Cr-Fe2-Ni2-Cu2</t>
-  </si>
-  <si>
     <t>Co-Cr-Fe-Ni-Cu-Al0.5-V0.8</t>
   </si>
   <si>
-    <t>Co-Cr-Fe0.6 -Ni-Al-Mo0.5</t>
+    <t>Amorphous</t>
+  </si>
+  <si>
+    <t>B2 + σ</t>
+  </si>
+  <si>
+    <t>BCC</t>
+  </si>
+  <si>
+    <t>BCC + σ</t>
+  </si>
+  <si>
+    <t>BCC1 + B2</t>
+  </si>
+  <si>
+    <t>Compounds</t>
   </si>
   <si>
     <t>FCC</t>
   </si>
   <si>
-    <t>BCC</t>
-  </si>
-  <si>
     <t>FCC + BCC</t>
   </si>
   <si>
-    <t>Amorphous</t>
-  </si>
-  <si>
-    <t>BCC + σ</t>
-  </si>
-  <si>
-    <t>B2 + σ</t>
-  </si>
-  <si>
-    <t>BCC1 + B2</t>
-  </si>
-  <si>
     <t>FCC + BCC + σ</t>
-  </si>
-  <si>
-    <t>Compounds</t>
   </si>
   <si>
     <t>HCP</t>
@@ -493,872 +496,1028 @@
       <c r="E1" t="s">
         <v>3</v>
       </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>55</v>
+        <v>5</v>
+      </c>
+      <c r="B2" t="n">
+        <v>3.0</v>
       </c>
       <c r="C2" t="s">
-        <v>95</v>
+        <v>56</v>
       </c>
       <c r="D2" t="s">
-        <v>129</v>
+        <v>96</v>
       </c>
       <c r="E2" t="s">
-        <v>138</v>
+        <v>130</v>
+      </c>
+      <c r="F2" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>56</v>
+        <v>6</v>
+      </c>
+      <c r="B3" t="n">
+        <v>5.0</v>
       </c>
       <c r="C3" t="s">
-        <v>96</v>
+        <v>57</v>
       </c>
       <c r="D3" t="s">
-        <v>129</v>
+        <v>57</v>
       </c>
       <c r="E3" t="s">
-        <v>129</v>
+        <v>130</v>
+      </c>
+      <c r="F3" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>56</v>
+        <v>7</v>
+      </c>
+      <c r="B4" t="n">
+        <v>5.0</v>
       </c>
       <c r="C4" t="s">
-        <v>97</v>
+        <v>58</v>
       </c>
       <c r="D4" t="s">
-        <v>130</v>
+        <v>58</v>
       </c>
       <c r="E4" t="s">
         <v>130</v>
       </c>
+      <c r="F4" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>57</v>
+        <v>8</v>
+      </c>
+      <c r="B5" t="n">
+        <v>3.0</v>
       </c>
       <c r="C5" t="s">
-        <v>98</v>
+        <v>59</v>
       </c>
       <c r="D5" t="s">
-        <v>131</v>
+        <v>97</v>
       </c>
       <c r="E5" t="s">
         <v>131</v>
       </c>
+      <c r="F5" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" t="s">
-        <v>57</v>
+        <v>9</v>
+      </c>
+      <c r="B6" t="n">
+        <v>1.0</v>
       </c>
       <c r="C6" t="s">
-        <v>99</v>
+        <v>60</v>
       </c>
       <c r="D6" t="s">
-        <v>130</v>
+        <v>98</v>
       </c>
       <c r="E6" t="s">
-        <v>131</v>
+        <v>132</v>
+      </c>
+      <c r="F6" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" t="s">
-        <v>58</v>
+        <v>10</v>
+      </c>
+      <c r="B7" t="n">
+        <v>2.0</v>
       </c>
       <c r="C7" t="s">
-        <v>100</v>
+        <v>61</v>
       </c>
       <c r="D7" t="s">
-        <v>129</v>
+        <v>99</v>
       </c>
       <c r="E7" t="s">
-        <v>131</v>
+        <v>132</v>
+      </c>
+      <c r="F7" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" t="s">
-        <v>59</v>
+        <v>11</v>
+      </c>
+      <c r="B8" t="n">
+        <v>2.0</v>
       </c>
       <c r="C8" t="s">
-        <v>101</v>
+        <v>62</v>
       </c>
       <c r="D8" t="s">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="E8" t="s">
-        <v>130</v>
+        <v>132</v>
+      </c>
+      <c r="F8" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" t="s">
-        <v>60</v>
+        <v>12</v>
+      </c>
+      <c r="B9" t="n">
+        <v>2.0</v>
       </c>
       <c r="C9" t="s">
-        <v>102</v>
+        <v>63</v>
       </c>
       <c r="D9" t="s">
-        <v>132</v>
+        <v>63</v>
       </c>
       <c r="E9" t="s">
-        <v>130</v>
+        <v>132</v>
+      </c>
+      <c r="F9" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" t="s">
-        <v>61</v>
+        <v>13</v>
+      </c>
+      <c r="B10" t="n">
+        <v>1.0</v>
       </c>
       <c r="C10" t="s">
-        <v>103</v>
+        <v>64</v>
       </c>
       <c r="D10" t="s">
-        <v>131</v>
+        <v>101</v>
       </c>
       <c r="E10" t="s">
-        <v>131</v>
+        <v>132</v>
+      </c>
+      <c r="F10" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" t="s">
-        <v>62</v>
+        <v>14</v>
+      </c>
+      <c r="B11" t="n">
+        <v>1.0</v>
       </c>
       <c r="C11" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D11" t="s">
-        <v>132</v>
+        <v>102</v>
       </c>
       <c r="E11" t="s">
+        <v>132</v>
+      </c>
+      <c r="F11" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" t="s">
-        <v>63</v>
+        <v>15</v>
+      </c>
+      <c r="B12" t="n">
+        <v>1.0</v>
       </c>
       <c r="C12" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D12" t="s">
-        <v>132</v>
+        <v>103</v>
       </c>
       <c r="E12" t="s">
-        <v>131</v>
+        <v>132</v>
+      </c>
+      <c r="F12" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" t="s">
-        <v>64</v>
+        <v>16</v>
+      </c>
+      <c r="B13" t="n">
+        <v>1.0</v>
       </c>
       <c r="C13" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D13" t="s">
-        <v>130</v>
+        <v>104</v>
       </c>
       <c r="E13" t="s">
-        <v>131</v>
+        <v>132</v>
+      </c>
+      <c r="F13" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" t="s">
-        <v>65</v>
+        <v>17</v>
+      </c>
+      <c r="B14" t="n">
+        <v>1.0</v>
       </c>
       <c r="C14" t="s">
+        <v>66</v>
+      </c>
+      <c r="D14" t="s">
         <v>104</v>
       </c>
-      <c r="D14" t="s">
-        <v>130</v>
-      </c>
       <c r="E14" t="s">
-        <v>130</v>
+        <v>132</v>
+      </c>
+      <c r="F14" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" t="s">
-        <v>65</v>
+        <v>18</v>
+      </c>
+      <c r="B15" t="n">
+        <v>1.0</v>
       </c>
       <c r="C15" t="s">
-        <v>105</v>
+        <v>66</v>
       </c>
       <c r="D15" t="s">
-        <v>130</v>
+        <v>104</v>
       </c>
       <c r="E15" t="s">
-        <v>130</v>
+        <v>132</v>
+      </c>
+      <c r="F15" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16" t="s">
-        <v>66</v>
+        <v>19</v>
+      </c>
+      <c r="B16" t="n">
+        <v>1.0</v>
       </c>
       <c r="C16" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D16" t="s">
-        <v>131</v>
+        <v>105</v>
       </c>
       <c r="E16" t="s">
-        <v>131</v>
+        <v>132</v>
+      </c>
+      <c r="F16" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C17" t="s">
         <v>67</v>
       </c>
-      <c r="C17" t="s">
-        <v>106</v>
-      </c>
       <c r="D17" t="s">
-        <v>133</v>
+        <v>105</v>
       </c>
       <c r="E17" t="s">
-        <v>133</v>
+        <v>132</v>
+      </c>
+      <c r="F17" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>20</v>
-      </c>
-      <c r="B18" t="s">
-        <v>68</v>
+        <v>21</v>
+      </c>
+      <c r="B18" t="n">
+        <v>3.0</v>
       </c>
       <c r="C18" t="s">
         <v>68</v>
       </c>
       <c r="D18" t="s">
-        <v>129</v>
+        <v>106</v>
       </c>
       <c r="E18" t="s">
-        <v>129</v>
+        <v>132</v>
+      </c>
+      <c r="F18" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C19" t="s">
         <v>69</v>
       </c>
-      <c r="C19" t="s">
-        <v>107</v>
-      </c>
       <c r="D19" t="s">
-        <v>129</v>
+        <v>69</v>
       </c>
       <c r="E19" t="s">
-        <v>129</v>
+        <v>132</v>
+      </c>
+      <c r="F19" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>22</v>
-      </c>
-      <c r="B20" t="s">
-        <v>61</v>
+        <v>23</v>
+      </c>
+      <c r="B20" t="n">
+        <v>4.0</v>
       </c>
       <c r="C20" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="D20" t="s">
-        <v>131</v>
+        <v>107</v>
       </c>
       <c r="E20" t="s">
-        <v>131</v>
+        <v>132</v>
+      </c>
+      <c r="F20" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>23</v>
-      </c>
-      <c r="B21" t="s">
-        <v>70</v>
+        <v>24</v>
+      </c>
+      <c r="B21" t="n">
+        <v>1.0</v>
       </c>
       <c r="C21" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D21" t="s">
-        <v>129</v>
+        <v>108</v>
       </c>
       <c r="E21" t="s">
-        <v>129</v>
+        <v>132</v>
+      </c>
+      <c r="F21" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>24</v>
-      </c>
-      <c r="B22" t="s">
-        <v>71</v>
+        <v>25</v>
+      </c>
+      <c r="B22" t="n">
+        <v>3.0</v>
       </c>
       <c r="C22" t="s">
-        <v>108</v>
+        <v>72</v>
       </c>
       <c r="D22" t="s">
-        <v>129</v>
+        <v>109</v>
       </c>
       <c r="E22" t="s">
-        <v>131</v>
+        <v>133</v>
+      </c>
+      <c r="F22" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>25</v>
-      </c>
-      <c r="B23" t="s">
-        <v>72</v>
+        <v>26</v>
+      </c>
+      <c r="B23" t="n">
+        <v>3.0</v>
       </c>
       <c r="C23" t="s">
-        <v>109</v>
+        <v>73</v>
       </c>
       <c r="D23" t="s">
-        <v>130</v>
+        <v>110</v>
       </c>
       <c r="E23" t="s">
-        <v>130</v>
+        <v>133</v>
+      </c>
+      <c r="F23" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>26</v>
-      </c>
-      <c r="B24" t="s">
-        <v>73</v>
+        <v>27</v>
+      </c>
+      <c r="B24" t="n">
+        <v>3.0</v>
       </c>
       <c r="C24" t="s">
-        <v>110</v>
+        <v>74</v>
       </c>
       <c r="D24" t="s">
-        <v>130</v>
+        <v>111</v>
       </c>
       <c r="E24" t="s">
-        <v>130</v>
+        <v>134</v>
+      </c>
+      <c r="F24" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>27</v>
-      </c>
-      <c r="B25" t="s">
-        <v>73</v>
+        <v>28</v>
+      </c>
+      <c r="B25" t="n">
+        <v>5.0</v>
       </c>
       <c r="C25" t="s">
-        <v>110</v>
+        <v>75</v>
       </c>
       <c r="D25" t="s">
-        <v>130</v>
+        <v>75</v>
       </c>
       <c r="E25" t="s">
-        <v>130</v>
+        <v>135</v>
+      </c>
+      <c r="F25" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>28</v>
-      </c>
-      <c r="B26" t="s">
-        <v>73</v>
+        <v>29</v>
+      </c>
+      <c r="B26" t="n">
+        <v>5.0</v>
       </c>
       <c r="C26" t="s">
-        <v>110</v>
+        <v>76</v>
       </c>
       <c r="D26" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="E26" t="s">
-        <v>130</v>
+        <v>136</v>
+      </c>
+      <c r="F26" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>29</v>
-      </c>
-      <c r="B27" t="s">
-        <v>74</v>
+        <v>30</v>
+      </c>
+      <c r="B27" t="n">
+        <v>1.0</v>
       </c>
       <c r="C27" t="s">
-        <v>111</v>
+        <v>60</v>
       </c>
       <c r="D27" t="s">
-        <v>130</v>
+        <v>113</v>
       </c>
       <c r="E27" t="s">
-        <v>130</v>
+        <v>136</v>
+      </c>
+      <c r="F27" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>30</v>
-      </c>
-      <c r="B28" t="s">
-        <v>74</v>
+        <v>31</v>
+      </c>
+      <c r="B28" t="n">
+        <v>2.0</v>
       </c>
       <c r="C28" t="s">
-        <v>111</v>
+        <v>77</v>
       </c>
       <c r="D28" t="s">
-        <v>130</v>
+        <v>114</v>
       </c>
       <c r="E28" t="s">
-        <v>130</v>
+        <v>136</v>
+      </c>
+      <c r="F28" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>31</v>
-      </c>
-      <c r="B29" t="s">
-        <v>75</v>
+        <v>32</v>
+      </c>
+      <c r="B29" t="n">
+        <v>2.0</v>
       </c>
       <c r="C29" t="s">
-        <v>112</v>
+        <v>78</v>
       </c>
       <c r="D29" t="s">
-        <v>130</v>
+        <v>78</v>
       </c>
       <c r="E29" t="s">
-        <v>131</v>
+        <v>136</v>
+      </c>
+      <c r="F29" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>32</v>
-      </c>
-      <c r="B30" t="s">
-        <v>76</v>
+        <v>33</v>
+      </c>
+      <c r="B30" t="n">
+        <v>1.0</v>
       </c>
       <c r="C30" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="D30" t="s">
-        <v>130</v>
+        <v>115</v>
       </c>
       <c r="E30" t="s">
-        <v>130</v>
+        <v>136</v>
+      </c>
+      <c r="F30" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>33</v>
-      </c>
-      <c r="B31" t="s">
-        <v>77</v>
+        <v>34</v>
+      </c>
+      <c r="B31" t="n">
+        <v>3.0</v>
       </c>
       <c r="C31" t="s">
-        <v>113</v>
+        <v>80</v>
       </c>
       <c r="D31" t="s">
-        <v>134</v>
+        <v>80</v>
       </c>
       <c r="E31" t="s">
-        <v>133</v>
+        <v>136</v>
+      </c>
+      <c r="F31" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>34</v>
-      </c>
-      <c r="B32" t="s">
-        <v>78</v>
+        <v>35</v>
+      </c>
+      <c r="B32" t="n">
+        <v>3.0</v>
       </c>
       <c r="C32" t="s">
-        <v>114</v>
+        <v>81</v>
       </c>
       <c r="D32" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="E32" t="s">
-        <v>130</v>
+        <v>136</v>
+      </c>
+      <c r="F32" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>35</v>
-      </c>
-      <c r="B33" t="s">
-        <v>79</v>
+        <v>36</v>
+      </c>
+      <c r="B33" t="n">
+        <v>3.0</v>
       </c>
       <c r="C33" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="D33" t="s">
-        <v>131</v>
+        <v>82</v>
       </c>
       <c r="E33" t="s">
-        <v>129</v>
+        <v>136</v>
+      </c>
+      <c r="F33" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>36</v>
-      </c>
-      <c r="B34" t="s">
-        <v>80</v>
+        <v>37</v>
+      </c>
+      <c r="B34" t="n">
+        <v>3.0</v>
       </c>
       <c r="C34" t="s">
-        <v>115</v>
+        <v>83</v>
       </c>
       <c r="D34" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
       <c r="E34" t="s">
-        <v>131</v>
+        <v>136</v>
+      </c>
+      <c r="F34" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>37</v>
-      </c>
-      <c r="B35" t="s">
-        <v>80</v>
+        <v>38</v>
+      </c>
+      <c r="B35" t="n">
+        <v>3.0</v>
       </c>
       <c r="C35" t="s">
-        <v>116</v>
+        <v>84</v>
       </c>
       <c r="D35" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="E35" t="s">
-        <v>131</v>
+        <v>136</v>
+      </c>
+      <c r="F35" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>38</v>
-      </c>
-      <c r="B36" t="s">
-        <v>81</v>
+        <v>39</v>
+      </c>
+      <c r="B36" t="n">
+        <v>1.0</v>
       </c>
       <c r="C36" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D36" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="E36" t="s">
-        <v>131</v>
+        <v>136</v>
+      </c>
+      <c r="F36" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>39</v>
-      </c>
-      <c r="B37" t="s">
-        <v>82</v>
+        <v>40</v>
+      </c>
+      <c r="B37" t="n">
+        <v>3.0</v>
       </c>
       <c r="C37" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="D37" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="E37" t="s">
-        <v>131</v>
+        <v>136</v>
+      </c>
+      <c r="F37" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>40</v>
-      </c>
-      <c r="B38" t="s">
-        <v>83</v>
+        <v>41</v>
+      </c>
+      <c r="B38" t="n">
+        <v>2.0</v>
       </c>
       <c r="C38" t="s">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="D38" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="E38" t="s">
-        <v>131</v>
+        <v>137</v>
+      </c>
+      <c r="F38" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>41</v>
-      </c>
-      <c r="B39" t="s">
-        <v>84</v>
+        <v>42</v>
+      </c>
+      <c r="B39" t="n">
+        <v>2.0</v>
       </c>
       <c r="C39" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D39" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="E39" t="s">
-        <v>131</v>
+        <v>137</v>
+      </c>
+      <c r="F39" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>42</v>
-      </c>
-      <c r="B40" t="s">
-        <v>80</v>
+        <v>43</v>
+      </c>
+      <c r="B40" t="n">
+        <v>2.0</v>
       </c>
       <c r="C40" t="s">
-        <v>117</v>
+        <v>87</v>
       </c>
       <c r="D40" t="s">
-        <v>131</v>
+        <v>87</v>
       </c>
       <c r="E40" t="s">
-        <v>131</v>
+        <v>137</v>
+      </c>
+      <c r="F40" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>43</v>
-      </c>
-      <c r="B41" t="s">
-        <v>85</v>
+        <v>44</v>
+      </c>
+      <c r="B41" t="n">
+        <v>2.0</v>
       </c>
       <c r="C41" t="s">
-        <v>118</v>
+        <v>86</v>
       </c>
       <c r="D41" t="s">
-        <v>129</v>
+        <v>86</v>
       </c>
       <c r="E41" t="s">
-        <v>129</v>
+        <v>137</v>
+      </c>
+      <c r="F41" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>44</v>
-      </c>
-      <c r="B42" t="s">
-        <v>86</v>
+        <v>45</v>
+      </c>
+      <c r="B42" t="n">
+        <v>3.0</v>
       </c>
       <c r="C42" t="s">
-        <v>119</v>
+        <v>88</v>
       </c>
       <c r="D42" t="s">
-        <v>131</v>
+        <v>88</v>
       </c>
       <c r="E42" t="s">
-        <v>131</v>
+        <v>137</v>
+      </c>
+      <c r="F42" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>45</v>
-      </c>
-      <c r="B43" t="s">
-        <v>87</v>
+        <v>46</v>
+      </c>
+      <c r="B43" t="n">
+        <v>1.0</v>
       </c>
       <c r="C43" t="s">
-        <v>120</v>
+        <v>89</v>
       </c>
       <c r="D43" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="E43" t="s">
-        <v>129</v>
+        <v>137</v>
+      </c>
+      <c r="F43" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>46</v>
-      </c>
-      <c r="B44" t="s">
-        <v>88</v>
+        <v>47</v>
+      </c>
+      <c r="B44" t="n">
+        <v>1.0</v>
       </c>
       <c r="C44" t="s">
-        <v>121</v>
+        <v>89</v>
       </c>
       <c r="D44" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="E44" t="s">
-        <v>131</v>
+        <v>137</v>
+      </c>
+      <c r="F44" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>47</v>
-      </c>
-      <c r="B45" t="s">
-        <v>69</v>
+        <v>48</v>
+      </c>
+      <c r="B45" t="n">
+        <v>2.0</v>
       </c>
       <c r="C45" t="s">
-        <v>122</v>
+        <v>90</v>
       </c>
       <c r="D45" t="s">
-        <v>129</v>
+        <v>90</v>
       </c>
       <c r="E45" t="s">
-        <v>129</v>
+        <v>137</v>
+      </c>
+      <c r="F45" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>48</v>
-      </c>
-      <c r="B46" t="s">
-        <v>89</v>
+        <v>49</v>
+      </c>
+      <c r="B46" t="n">
+        <v>3.0</v>
       </c>
       <c r="C46" t="s">
-        <v>123</v>
+        <v>91</v>
       </c>
       <c r="D46" t="s">
-        <v>130</v>
+        <v>91</v>
       </c>
       <c r="E46" t="s">
-        <v>130</v>
+        <v>137</v>
+      </c>
+      <c r="F46" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>49</v>
-      </c>
-      <c r="B47" t="s">
-        <v>90</v>
+        <v>50</v>
+      </c>
+      <c r="B47" t="n">
+        <v>2.0</v>
       </c>
       <c r="C47" t="s">
-        <v>124</v>
+        <v>92</v>
       </c>
       <c r="D47" t="s">
-        <v>131</v>
+        <v>92</v>
       </c>
       <c r="E47" t="s">
-        <v>131</v>
+        <v>137</v>
+      </c>
+      <c r="F47" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>50</v>
-      </c>
-      <c r="B48" t="s">
-        <v>91</v>
+        <v>51</v>
+      </c>
+      <c r="B48" t="n">
+        <v>1.0</v>
       </c>
       <c r="C48" t="s">
+        <v>89</v>
+      </c>
+      <c r="D48" t="s">
         <v>125</v>
       </c>
-      <c r="D48" t="s">
-        <v>131</v>
-      </c>
       <c r="E48" t="s">
-        <v>131</v>
+        <v>137</v>
+      </c>
+      <c r="F48" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>51</v>
-      </c>
-      <c r="B49" t="s">
-        <v>90</v>
+        <v>52</v>
+      </c>
+      <c r="B49" t="n">
+        <v>3.0</v>
       </c>
       <c r="C49" t="s">
+        <v>93</v>
+      </c>
+      <c r="D49" t="s">
         <v>126</v>
       </c>
-      <c r="D49" t="s">
-        <v>129</v>
-      </c>
       <c r="E49" t="s">
-        <v>129</v>
+        <v>137</v>
+      </c>
+      <c r="F49" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>52</v>
-      </c>
-      <c r="B50" t="s">
-        <v>92</v>
+        <v>53</v>
+      </c>
+      <c r="B50" t="n">
+        <v>3.0</v>
       </c>
       <c r="C50" t="s">
+        <v>85</v>
+      </c>
+      <c r="D50" t="s">
         <v>127</v>
       </c>
-      <c r="D50" t="s">
-        <v>136</v>
-      </c>
       <c r="E50" t="s">
-        <v>131</v>
+        <v>137</v>
+      </c>
+      <c r="F50" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>53</v>
-      </c>
-      <c r="B51" t="s">
-        <v>93</v>
+        <v>54</v>
+      </c>
+      <c r="B51" t="n">
+        <v>3.0</v>
       </c>
       <c r="C51" t="s">
+        <v>94</v>
+      </c>
+      <c r="D51" t="s">
         <v>128</v>
       </c>
-      <c r="D51" t="s">
-        <v>133</v>
-      </c>
       <c r="E51" t="s">
-        <v>133</v>
+        <v>137</v>
+      </c>
+      <c r="F51" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>54</v>
-      </c>
-      <c r="B52" t="s">
-        <v>94</v>
+        <v>55</v>
+      </c>
+      <c r="B52" t="n">
+        <v>2.0</v>
       </c>
       <c r="C52" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D52" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="E52" t="s">
-        <v>129</v>
+        <v>138</v>
+      </c>
+      <c r="F52" t="s">
+        <v>137</v>
       </c>
     </row>
   </sheetData>

</xml_diff>